<commit_message>
Better data cleaning, more efficient code and also prediction (not done)
</commit_message>
<xml_diff>
--- a/stance_sample.xlsx
+++ b/stance_sample.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>result_clean</t>
+          <t>result</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -512,7 +512,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -612,7 +612,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -628,7 +628,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -662,7 +662,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -768,7 +768,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -817,7 +817,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -843,7 +843,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>abgelehnt</t>
+          <t>Abgelehnt</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -901,7 +901,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -916,7 +916,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -936,7 +936,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -966,7 +966,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -996,7 +996,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>angenommen</t>
+          <t>Angenommen</t>
         </is>
       </c>
     </row>

</xml_diff>